<commit_message>
Updated files with spec and dich
</commit_message>
<xml_diff>
--- a/header_files/pmpart_headers.xlsx
+++ b/header_files/pmpart_headers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shann\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C30B31-9095-42C2-AA2D-2D2FC813D6CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D05B8A0-3F04-4733-9162-B68CFFE2CFB1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="3360" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="128">
   <si>
     <t>date</t>
   </si>
@@ -412,6 +412,9 @@
   </si>
   <si>
     <t>barium_mdl</t>
+  </si>
+  <si>
+    <t>spec_pm2_5</t>
   </si>
 </sst>
 </file>
@@ -755,7 +758,7 @@
   <dimension ref="A1:AY4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -920,7 +923,7 @@
         <v>120</v>
       </c>
       <c r="G2" t="s">
-        <v>78</v>
+        <v>127</v>
       </c>
       <c r="I2" t="s">
         <v>49</v>

</xml_diff>